<commit_message>
Files & Folders Added Or Created In 1.5 Months
</commit_message>
<xml_diff>
--- a/Bhumika Mam (Home Practice)/Excel Practice(Home) New.xlsx
+++ b/Bhumika Mam (Home Practice)/Excel Practice(Home) New.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achyut Sharma\Documents\Data Sem 5\Bhumika Mam (Home Practice)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5C632E-41BD-4B97-8310-F8D6A006B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6C02DF-794E-4C90-B7F2-1D6381507C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5DBA3395-1028-448A-80F9-213C0DDA284A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{5DBA3395-1028-448A-80F9-213C0DDA284A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
+    <sheet name="Practice Work 6 Aug" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>count</t>
   </si>
@@ -244,6 +267,57 @@
   </si>
   <si>
     <t>upper limi</t>
+  </si>
+  <si>
+    <t>Obs.</t>
+  </si>
+  <si>
+    <t>N(no.of obs)</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Asc.obs.</t>
+  </si>
+  <si>
+    <t>Asc.Obs.</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Asc.Obs</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>As.Obs</t>
+  </si>
+  <si>
+    <t>As.Obs.</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Asc obs</t>
+  </si>
+  <si>
+    <t>Asc</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roll No(X)</t>
+  </si>
+  <si>
+    <t>Marks.(F)</t>
   </si>
 </sst>
 </file>
@@ -2446,7 +2520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4187230-8FBB-4592-BE1D-7C829685C8FB}">
   <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
@@ -4376,7 +4450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7AA84B-E10E-4D7B-9C8D-CA7797EF3C76}">
   <dimension ref="A2:R102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
@@ -4963,7 +5037,7 @@
         <v>46</v>
       </c>
       <c r="G54">
-        <f t="shared" ref="F54:G54" si="2">H51/F51</f>
+        <f t="shared" ref="G54" si="2">H51/F51</f>
         <v>0</v>
       </c>
       <c r="J54">
@@ -5285,4 +5359,993 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE89C6B-7696-47E5-A1BC-DC6D76CD5E84}">
+  <dimension ref="B2:R103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="12" width="11.77734375" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2">
+        <f>COUNT(_xlfn.ANCHORARRAY(O3))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" cm="1">
+        <f t="array" ref="C3:C12">_xlfn._xlws.SORT(B3:B12,,1,)</f>
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3">
+        <f>COUNT(B3:B12)</f>
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>58</v>
+      </c>
+      <c r="O3" cm="1">
+        <f t="array" ref="O3:O12">_xlfn._xlws.SORT(N3:N12,,1,)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>41</v>
+      </c>
+      <c r="O4">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4">
+        <f>SUM(_xlfn.ANCHORARRAY(O3))</f>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5">
+        <f>SUM(B3:B12)</f>
+        <v>148</v>
+      </c>
+      <c r="N5">
+        <v>25</v>
+      </c>
+      <c r="O5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>77</v>
+      </c>
+      <c r="O6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <f>(F5/F3)</f>
+        <v>14.8</v>
+      </c>
+      <c r="N7">
+        <v>22</v>
+      </c>
+      <c r="O7">
+        <v>54</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7">
+        <f>(R4/R2)</f>
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>54</v>
+      </c>
+      <c r="O8">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <f>MEDIAN(C6:C7)</f>
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>58</v>
+      </c>
+      <c r="O9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="N10">
+        <v>24</v>
+      </c>
+      <c r="O10">
+        <v>58</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>70</v>
+      </c>
+      <c r="R10">
+        <f>(O7+O8)/2</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="N11">
+        <v>86</v>
+      </c>
+      <c r="O11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>54</v>
+      </c>
+      <c r="N12">
+        <v>54</v>
+      </c>
+      <c r="O12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14">
+        <f>COUNT(_xlfn.ANCHORARRAY(J15))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15:J24">_xlfn._xlws.SORT(I15:I24,,1,)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>25</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>26</v>
+      </c>
+      <c r="J17">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17">
+        <f>SUM(_xlfn.ANCHORARRAY(J15))</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>89</v>
+      </c>
+      <c r="J18">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>74</v>
+      </c>
+      <c r="J19">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>41</v>
+      </c>
+      <c r="J20">
+        <v>57</v>
+      </c>
+      <c r="K20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(J15))</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>25</v>
+      </c>
+      <c r="J21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>87</v>
+      </c>
+      <c r="J22">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23">
+        <f>COUNT(_xlfn.ANCHORARRAY(F24))</f>
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>84</v>
+      </c>
+      <c r="J23">
+        <v>87</v>
+      </c>
+      <c r="K23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(J15))</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24" cm="1">
+        <f t="array" ref="F24:F33">_xlfn._xlws.SORT(E24:E33,,1,)</f>
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>57</v>
+      </c>
+      <c r="J24">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>33</v>
+      </c>
+      <c r="F25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>96</v>
+      </c>
+      <c r="F26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>13</v>
+      </c>
+      <c r="F27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>78</v>
+      </c>
+      <c r="F28">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(F24))</f>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>54</v>
+      </c>
+      <c r="F29">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>26</v>
+      </c>
+      <c r="F30">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>35</v>
+      </c>
+      <c r="F31">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>95</v>
+      </c>
+      <c r="F32">
+        <v>95</v>
+      </c>
+      <c r="G32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(F24))</f>
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>55</v>
+      </c>
+      <c r="F33">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36">
+        <f>COUNT(_xlfn.ANCHORARRAY(F37))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>85</v>
+      </c>
+      <c r="F37" cm="1">
+        <f t="array" ref="F37:F46">_xlfn._xlws.SORT(E37:E46)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>26</v>
+      </c>
+      <c r="F38">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>24</v>
+      </c>
+      <c r="F39">
+        <v>33</v>
+      </c>
+      <c r="G39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(F37))</f>
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>98</v>
+      </c>
+      <c r="F40">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>88</v>
+      </c>
+      <c r="F41">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>74</v>
+      </c>
+      <c r="F42">
+        <v>74</v>
+      </c>
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(F37))</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>58</v>
+      </c>
+      <c r="F43">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>96</v>
+      </c>
+      <c r="F44">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>33</v>
+      </c>
+      <c r="F45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>66</v>
+      </c>
+      <c r="F46">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50">
+        <f>COUNT(_xlfn.ANCHORARRAY(C51))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51" cm="1">
+        <f t="array" ref="C51:C60">_xlfn._xlws.SORT(B51:B60)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>88</v>
+      </c>
+      <c r="C52">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>74</v>
+      </c>
+      <c r="C53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>58</v>
+      </c>
+      <c r="C54">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(C51))</f>
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>78</v>
+      </c>
+      <c r="C55">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>52</v>
+      </c>
+      <c r="C56">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>65</v>
+      </c>
+      <c r="C58">
+        <v>74</v>
+      </c>
+      <c r="D58" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(C51))</f>
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>21</v>
+      </c>
+      <c r="C60">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H61" t="s">
+        <v>75</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" t="s">
+        <v>78</v>
+      </c>
+      <c r="K61">
+        <f>COUNT(_xlfn.ANCHORARRAY(I62))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H62">
+        <v>9</v>
+      </c>
+      <c r="I62" cm="1">
+        <f t="array" ref="I62:I68">_xlfn._xlws.SORT(H62:H68)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H63">
+        <v>7</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H65">
+        <v>7</v>
+      </c>
+      <c r="I65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H67">
+        <v>4</v>
+      </c>
+      <c r="I67">
+        <v>7</v>
+      </c>
+      <c r="J67" t="s">
+        <v>46</v>
+      </c>
+      <c r="K67">
+        <f>MEDIAN(I62:I68)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H68">
+        <v>7</v>
+      </c>
+      <c r="I68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H70" t="s">
+        <v>75</v>
+      </c>
+      <c r="I70" t="s">
+        <v>78</v>
+      </c>
+      <c r="J70">
+        <f>COUNT(H71:H75)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72" t="s">
+        <v>46</v>
+      </c>
+      <c r="J72">
+        <f>MEDIAN(H71:H75)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78">
+        <f>COUNT(_xlfn.ANCHORARRAY(D79))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>12</v>
+      </c>
+      <c r="D79" cm="1">
+        <f t="array" ref="D79:D85">_xlfn._xlws.SORT(C79:C85)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>52</v>
+      </c>
+      <c r="D80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>59</v>
+      </c>
+      <c r="D81">
+        <v>35</v>
+      </c>
+      <c r="E81" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81">
+        <f>MEDIAN(_xlfn.ANCHORARRAY(D79))</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>65</v>
+      </c>
+      <c r="D82">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>25</v>
+      </c>
+      <c r="D83">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>62</v>
+      </c>
+      <c r="D84">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>35</v>
+      </c>
+      <c r="D85">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>83</v>
+      </c>
+      <c r="D93" t="s">
+        <v>84</v>
+      </c>
+      <c r="F93" t="s">
+        <v>73</v>
+      </c>
+      <c r="G93">
+        <f>COUNT(C94:C103)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>87</v>
+      </c>
+      <c r="F95" t="s">
+        <v>53</v>
+      </c>
+      <c r="G95">
+        <f>SUM(D94:D103)</f>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <v>4</v>
+      </c>
+      <c r="D97">
+        <v>84</v>
+      </c>
+      <c r="F97" t="s">
+        <v>79</v>
+      </c>
+      <c r="G97">
+        <f>(G95/G93)</f>
+        <v>66.2</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <v>5</v>
+      </c>
+      <c r="D98">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <v>6</v>
+      </c>
+      <c r="D99">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <v>7</v>
+      </c>
+      <c r="D100">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <v>8</v>
+      </c>
+      <c r="D101">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <v>9</v>
+      </c>
+      <c r="D102">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>